<commit_message>
experiment spits out excel-able table
</commit_message>
<xml_diff>
--- a/reaction experiments.xlsx
+++ b/reaction experiments.xlsx
@@ -16,93 +16,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
-  <si>
-    <t>Reaction equilibrium tests</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>~1</t>
-  </si>
-  <si>
-    <t>Rxn</t>
-  </si>
-  <si>
-    <t>A+B-&gt;C+D</t>
-  </si>
-  <si>
-    <t>dhf</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (-10) + (-10) -&gt; (-11) + (-11)</t>
-  </si>
-  <si>
-    <t>(.25) + (.25) &amp;&amp; (.25) + (.25)</t>
-  </si>
-  <si>
-    <t>fracs calc</t>
-  </si>
-  <si>
-    <t>K calc</t>
-  </si>
-  <si>
-    <t>K obs</t>
-  </si>
-  <si>
-    <t>fracs obs</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Woo!</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (-10) + (-10) -&gt; (-10) + (-10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.5-2.5, avg ~1.9</t>
-  </si>
-  <si>
-    <t>(.20) + (.20) &amp;&amp; (.30) + (.30)</t>
-  </si>
-  <si>
-    <t>(.21) + (.21) &amp;&amp; (.29) + (.29)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eq const propto frac ratio sqr, so very sensitive to small x change.  Good though. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (-10) + (-10) -&gt; (-13) + (-13)</t>
-  </si>
-  <si>
-    <t>Temp</t>
-  </si>
-  <si>
-    <t>(.114) + (.114) &amp;&amp; (.386) + (.386)</t>
-  </si>
-  <si>
-    <t>(.5) &amp;&amp; (.5)</t>
-  </si>
-  <si>
-    <t>(.4) &amp;&amp; (.6)</t>
-  </si>
-  <si>
-    <t>(.228) &amp;&amp; (.772)</t>
-  </si>
-  <si>
-    <t>(.28) &amp;&amp; (.72)</t>
-  </si>
-  <si>
-    <t>(.14) + (.14) &amp;&amp; (.36) + (.36)</t>
-  </si>
-  <si>
-    <t>~6.2</t>
-  </si>
-  <si>
-    <t>Boolean prob func</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>eaf</t>
+  </si>
+  <si>
+    <t>ear</t>
+  </si>
+  <si>
+    <t>hfa</t>
+  </si>
+  <si>
+    <t>hfb</t>
+  </si>
+  <si>
+    <t>hfc</t>
+  </si>
+  <si>
+    <t>hfd</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>nb</t>
+  </si>
+  <si>
+    <t>nc</t>
+  </si>
+  <si>
+    <t>nd</t>
+  </si>
+  <si>
+    <t>prod</t>
+  </si>
+  <si>
+    <t>predicted</t>
+  </si>
+  <si>
+    <t>probFunc: eHit &gt; Ea ? 1 : 0</t>
+  </si>
+  <si>
+    <t>probFunc: eHit &gt; 1.2 * Ea ? 1 : 0</t>
   </si>
 </sst>
 </file>
@@ -434,161 +389,294 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:P20"/>
+  <dimension ref="A3:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="4" max="4" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.21875" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="2" spans="2:16">
-      <c r="B2" t="s">
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:16">
-      <c r="B5" t="s">
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="J4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" t="s">
         <v>9</v>
       </c>
-      <c r="G5" t="s">
+      <c r="N4" t="s">
         <v>10</v>
       </c>
-      <c r="I5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="O4" t="s">
         <v>11</v>
       </c>
-      <c r="P5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16">
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="5" spans="1:15">
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7">
-        <v>298</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" t="s">
-        <v>7</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>-10</v>
+      </c>
+      <c r="F5">
+        <v>-10</v>
+      </c>
+      <c r="G5">
+        <v>-13</v>
+      </c>
+      <c r="H5">
+        <v>-13</v>
+      </c>
+      <c r="J5">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="K5">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="L5">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="M5">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="N5">
+        <f>SUM(L5:M5)</f>
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="O5">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>-10</v>
+      </c>
+      <c r="F6">
+        <v>-10</v>
+      </c>
+      <c r="G6">
+        <v>-12</v>
+      </c>
+      <c r="H6">
+        <v>-12</v>
+      </c>
+      <c r="J6">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="K6">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="L6">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="M6">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="N6">
+        <f>SUM(L6:M6)</f>
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="O6">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:16">
-      <c r="I8" t="s">
-        <v>22</v>
-      </c>
-      <c r="P8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16">
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
+    <row r="11" spans="1:15">
+      <c r="C11">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
-        <v>6</v>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>-10</v>
+      </c>
+      <c r="F11">
+        <v>-10</v>
+      </c>
+      <c r="G11">
+        <v>-13</v>
+      </c>
+      <c r="H11">
+        <v>-13</v>
+      </c>
+      <c r="J11">
+        <v>0.126</v>
+      </c>
+      <c r="K11">
+        <v>0.126</v>
+      </c>
+      <c r="L11">
+        <v>0.374</v>
+      </c>
+      <c r="M11">
+        <v>0.374</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ref="N7:N14" si="0">SUM(L11:M11)</f>
+        <v>0.748</v>
+      </c>
+      <c r="O11">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
       </c>
       <c r="E12">
-        <v>298</v>
+        <v>-10</v>
       </c>
       <c r="F12">
-        <v>2.2410000000000001</v>
-      </c>
-      <c r="G12" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" t="s">
-        <v>16</v>
-      </c>
-      <c r="L12" t="s">
-        <v>17</v>
-      </c>
-      <c r="P12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16">
-      <c r="I13" t="s">
-        <v>23</v>
-      </c>
-      <c r="P13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16">
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
+        <v>-10</v>
+      </c>
+      <c r="G12">
+        <v>-12</v>
+      </c>
+      <c r="H12">
+        <v>-12</v>
+      </c>
+      <c r="J12">
+        <v>0.154</v>
+      </c>
+      <c r="K12">
+        <v>0.154</v>
+      </c>
+      <c r="L12">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="M12">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>0.69</v>
+      </c>
+      <c r="O12">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="C13">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19">
-        <v>298</v>
-      </c>
-      <c r="F19">
-        <v>11.25</v>
-      </c>
-      <c r="G19" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" t="s">
-        <v>26</v>
-      </c>
-      <c r="P19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16">
-      <c r="I20" t="s">
-        <v>24</v>
-      </c>
-      <c r="L20" t="s">
-        <v>25</v>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>-10</v>
+      </c>
+      <c r="F13">
+        <v>-10</v>
+      </c>
+      <c r="G13">
+        <v>-11</v>
+      </c>
+      <c r="H13">
+        <v>-11</v>
+      </c>
+      <c r="J13">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="K13">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="L13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="M13">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="O13">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>-10</v>
+      </c>
+      <c r="F14">
+        <v>-10</v>
+      </c>
+      <c r="G14">
+        <v>-10</v>
+      </c>
+      <c r="H14">
+        <v>-10</v>
+      </c>
+      <c r="J14">
+        <v>0.25</v>
+      </c>
+      <c r="K14">
+        <v>0.25</v>
+      </c>
+      <c r="L14">
+        <v>0.25</v>
+      </c>
+      <c r="M14">
+        <v>0.25</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="O14">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>